<commit_message>
Calculate the distribuction of cross-origin frame chains
</commit_message>
<xml_diff>
--- a/result_handler/results.xlsx
+++ b/result_handler/results.xlsx
@@ -8,19 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lwyeluo/Workspaces/lab-project/browser/tim-evaluate/result_handler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1DD2BC-E862-3E4E-9F6F-AF1CD1F9B5B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A5071C-F9A8-0242-8C91-E5C275964BAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="2" xr2:uid="{A38FA40B-9AA0-234E-B7A1-9A1E5346C45F}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="3" xr2:uid="{A38FA40B-9AA0-234E-B7A1-9A1E5346C45F}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
     <sheet name="distribution" sheetId="2" r:id="rId2"/>
     <sheet name="cross-origin domains" sheetId="3" r:id="rId3"/>
+    <sheet name="distribution of cross-origin" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">distribution!$A$2:$A$19</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">distribution!$B$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">distribution!$B$2:$B$19</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">distribution!$C$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">distribution!$C$2:$C$19</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">distribution!$A$2:$A$19</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">distribution!$B$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">distribution!$B$2:$B$19</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">distribution!$C$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">distribution!$C$2:$C$19</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">distribution!$B$2:$B$19</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">distribution!$A$2:$A$19</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">distribution!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">distribution!$B$2:$B$19</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">distribution!$C$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">distribution!$C$2:$C$19</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">distribution!$A$2:$A$19</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">distribution!$B$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="820">
   <si>
     <t>rank</t>
   </si>
@@ -2336,16 +2352,186 @@
   </si>
   <si>
     <t>#cross_origin</t>
+  </si>
+  <si>
+    <t>lengthOfCrossOriginFC</t>
+  </si>
+  <si>
+    <t>largestCrossOriginFC</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>-5:6_https://a3698060313.cdn.optimizely.com/-5:3_https://outlook.live.com/</t>
+  </si>
+  <si>
+    <t>-5:3_https://www.yahoo.co.jp/-5:5_https://s.yimg.jp/-5:3_https://www.yahoo.co.jp/</t>
+  </si>
+  <si>
+    <t>-5:6_https://www.microsoftstore.com.cn/-5:3_https://www.microsoft.com/</t>
+  </si>
+  <si>
+    <t>-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/-5:3_https://www.naver.com/-5:7_https://nv.veta.naver.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://vars.hotjar.com/-5:3_https://wordpress.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://images-eu.ssl-images-amazon.com/-5:3_https://www.amazon.de/</t>
+  </si>
+  <si>
+    <t>-5:6_https://images-eu.ssl-images-amazon.com/-5:3_https://www.amazon.co.uk/</t>
+  </si>
+  <si>
+    <t>-5:6_https://www.craigslist.org/-5:3_https://beijing.craigslist.org/-5:6_https://www.craigslist.org/-5:3_https://beijing.craigslist.org/-5:6_https://www.craigslist.org/-5:3_https://beijing.craigslist.org/-5:6_https://www.craigslist.org/-5:3_https://beijing.craigslist.org/-5:6_https://www.craigslist.org/-5:3_https://beijing.craigslist.org/</t>
+  </si>
+  <si>
+    <t>-5:8_https://vars.hotjar.com/-5:3_https://www.spotify.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://a125375509.cdn.optimizely.com/-5:3_https://edition.cnn.com/</t>
+  </si>
+  <si>
+    <t>-5:8_https://8666735.fls.doubleclick.net/-5:3_https://www.etsy.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://tm.uol.com.br/-5:3_https://www.uol.com.br/</t>
+  </si>
+  <si>
+    <t>-5:9_https://music.douban.com/-5:3_https://www.douban.com/</t>
+  </si>
+  <si>
+    <t>-5:7_https://6372968.fls.doubleclick.net/-5:3_https://www.yelp.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://espn.demdex.net/-5:3_https://www.espncricinfo.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://elsevier.demdex.net/-5:3_https://www.sciencedirect.com/</t>
+  </si>
+  <si>
+    <t>-5:12_https://rutrk.org/-5:14_https://rutracker.org/-5:11_https://rutracker.org/-5:14_https://rutracker.org/-5:11_https://rutracker.org/-5:14_https://rutracker.org/-5:11_https://rutracker.org/-5:14_https://rutracker.org/-5:11_https://rutracker.org/-5:14_https://rutracker.org/-5:11_https://rutracker.org/-5:14_https://rutracker.org/</t>
+  </si>
+  <si>
+    <t>-5:5_https://id.rambler.ru/-5:3_https://www.rambler.ru/</t>
+  </si>
+  <si>
+    <t>-5:8_https://mscom.demdex.net/-5:3_https://www.xbox.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://bestbuy.demdex.net/-5:3_https://www.bestbuy.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://images-na.ssl-images-amazon.com/-5:3_https://www.amazon.ca/</t>
+  </si>
+  <si>
+    <t>-5:6_https://polaris.xfinity.com/-5:3_https://www.xfinity.com/</t>
+  </si>
+  <si>
+    <t>-5:7_https://vars.hotjar.com/-5:3_https://www.mgid.com/</t>
+  </si>
+  <si>
+    <t>-5:5_https://a11179690159.cdn.optimizely.com/-5:3_https://slack.com/</t>
+  </si>
+  <si>
+    <t>-5:4_https://vars.hotjar.com/-5:3_https://www.outbrain.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://sync.adkernel.com/-5:3_https://myanimelist.net/</t>
+  </si>
+  <si>
+    <t>-5:6_https://images-cn.ssl-images-amazon.com/-5:3_https://www.amazon.cn/</t>
+  </si>
+  <si>
+    <t>-6:6_https://apps.game.qq.com/-6:3_https://lol.qq.com/</t>
+  </si>
+  <si>
+    <t>-5:7_https://tpc.googlesyndication.com/-5:3_https://sourceforge.net/-5:9_https://tpc.googlesyndication.com/-5:7_https://tpc.googlesyndication.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://slickdeals.demdex.net/-5:3_https://slickdeals.net/</t>
+  </si>
+  <si>
+    <t>-5:6_https://a1859010085.cdn.optimizely.com/-5:3_https://www.springer.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://hdfcbank.demdex.net/-5:3_https://www.hdfcbank.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://symantec.demdex.net/-5:3_https://cn.norton.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://elsevier.demdex.net/-5:3_https://www.elsevier.com/</t>
+  </si>
+  <si>
+    <t>-6:5_https://a3698060313.cdn.optimizely.com/-6:3_https://products.office.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://a112699136.cdn.optimizely.com/-5:3_https://www.zendesk.com/</t>
+  </si>
+  <si>
+    <t>-5:7_https://tpc.googlesyndication.com/-5:3_https://hatenablog.com/</t>
+  </si>
+  <si>
+    <t>-5:7_https://lowescompaniesinc.demdex.net/-5:3_https://www.lowes.com/</t>
+  </si>
+  <si>
+    <t>-5:6_https://a.adtng.com/-5:3_https://nhentai.net/</t>
+  </si>
+  <si>
+    <t>-5:6_https://a166211981.cdn.optimizely.com/-5:3_https://www.intuit.com/</t>
+  </si>
+  <si>
+    <t>-5:4_https://consentcdn.cookiebot.com/-5:3_https://themeforest.net/</t>
+  </si>
+  <si>
+    <t>-6:4_https://a8270235338.cdn.optimizely.com/-6:3_https://www.blizzard.com/</t>
+  </si>
+  <si>
+    <t>-5:7_https://webmd.demdex.net/-5:3_https://www.webmd.com/</t>
+  </si>
+  <si>
+    <t>onload</t>
+  </si>
+  <si>
+    <t>document.domain</t>
+  </si>
+  <si>
+    <t>onreadystatechange</t>
+  </si>
+  <si>
+    <t>onscroll</t>
+  </si>
+  <si>
+    <t>onload/onreadystatechange</t>
+  </si>
+  <si>
+    <t>live.com,microsoft.com,wordpress.com,amazon.de,amazon.co.uk,spotify.com,cnn.com,etsy.com,uol.com.br,douban.com,yelp.com,www.espncricinfo.com,www.sciencedirect.com,rambler.ru,xbox.com,bestbuy.com,amazon.ca,www.xfinity.com,mgid.com,slack.com,outbrain.com,myanimelist.net,amazon.cn,leagueoflegends.com,slickdeals.net,springer.com,files.wordpress.com,hdfcbank.com,norton.com,elsevier.com,office365.com,zendesk.com,hatenablog.com,lowes.com,nhentai.net,intuit.com,themeforest.net,battle.net,webmd.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2371,11 +2557,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3062,6 +3255,988 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>distribution!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#domains</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>distribution!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>distribution!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0695-9743-8FAD-EE00857C48F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="1737032256"/>
+        <c:axId val="1669036480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1737032256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Maximum length of frame chain for tasks</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1669036480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1669036480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>number of domains</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1737032256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'distribution of cross-origin'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#domains</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'distribution of cross-origin'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'distribution of cross-origin'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF91-4047-B52D-32B1E3BDF824}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="1737032256"/>
+        <c:axId val="1669036480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1737032256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Maximum length of cross-origin frame chain for tasks</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1669036480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1669036480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>number of domains</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1737032256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
@@ -3286,6 +4461,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4331,20 +5586,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4371,16 +6632,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -4416,7 +6677,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10775950" y="4121150"/>
+              <a:off x="10179050" y="4908550"/>
               <a:ext cx="5594350" cy="2914650"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4445,6 +6706,87 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4432300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56365C64-04CD-1F47-8783-E038B2B362F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85E567DC-9F0A-504C-ADA1-A35BA35D56D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4749,8 +7091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D10F5A-9403-844E-9DB6-628B74D1C612}">
   <dimension ref="A1:Z503"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28496,7 +30838,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28847,371 +31189,876 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDC9EFE-7FAE-1341-9EA9-E8B8A6EB11B7}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="103.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="C1" t="s">
+        <v>769</v>
+      </c>
+      <c r="D1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>771</v>
+      </c>
+      <c r="D2" s="1">
         <v>43643.167060185187</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="9">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>772</v>
+      </c>
+      <c r="D3" s="10">
         <v>43643.177094907405</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F3" s="8" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>773</v>
+      </c>
+      <c r="D4" s="1">
         <v>43643.189236111109</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="F4" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="6">
+        <v>29</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>774</v>
+      </c>
+      <c r="D5" s="7">
         <v>43643.19259259259</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="F5" s="5" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>775</v>
+      </c>
+      <c r="D6" s="1">
         <v>43643.21025462963</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>776</v>
+      </c>
+      <c r="D7" s="1">
         <v>43643.236701388887</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="F7" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>777</v>
+      </c>
+      <c r="D8" s="1">
         <v>43643.243993055556</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="F8" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="6">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="D9" s="7">
         <v>43643.251099537039</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="F9" s="5" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>779</v>
+      </c>
+      <c r="D10" s="1">
         <v>43643.257291666669</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="F10" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>142</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>780</v>
+      </c>
+      <c r="D11" s="1">
         <v>43643.271979166668</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="F11" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>781</v>
+      </c>
+      <c r="D12" s="1">
         <v>43643.281643518516</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="F12" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>782</v>
+      </c>
+      <c r="D13" s="1">
         <v>43643.305474537039</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="F13" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>783</v>
+      </c>
+      <c r="D14" s="1">
         <v>43643.329548611109</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="F14" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>784</v>
+      </c>
+      <c r="D15" s="1">
         <v>43643.346550925926</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="F15" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>216</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="4">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>785</v>
+      </c>
+      <c r="D16" s="1">
         <v>43643.348171296297</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="F16" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>244</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>786</v>
+      </c>
+      <c r="D17" s="1">
         <v>43643.378298611111</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="F17" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="9">
+        <v>12</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="D18" s="10">
         <v>43643.38380787037</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="F18" s="8" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>264</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="4">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>788</v>
+      </c>
+      <c r="D19" s="1">
         <v>43643.398414351854</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="F19" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>284</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="4">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>789</v>
+      </c>
+      <c r="D20" s="1">
         <v>43643.413807870369</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="F20" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>286</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>790</v>
+      </c>
+      <c r="D21" s="1">
         <v>43643.416562500002</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="F21" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>290</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="4">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>791</v>
+      </c>
+      <c r="D22" s="1">
         <v>43643.419537037036</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="F22" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>322</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>792</v>
+      </c>
+      <c r="D23" s="1">
         <v>43643.450891203705</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="F23" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>332</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B24" s="4">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>793</v>
+      </c>
+      <c r="D24" s="1">
         <v>43643.457604166666</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="F24" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>410</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B25" s="4">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>794</v>
+      </c>
+      <c r="D25" s="1">
         <v>43643.512881944444</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="F25" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>430</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B26" s="4">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>795</v>
+      </c>
+      <c r="D26" s="1">
         <v>43643.533993055556</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="F26" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>438</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B27" s="4">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>796</v>
+      </c>
+      <c r="D27" s="1">
         <v>43643.543645833335</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="F27" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>456</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>797</v>
+      </c>
+      <c r="D28" s="1">
         <v>43643.563449074078</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="F28" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>462</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B29" s="4">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>798</v>
+      </c>
+      <c r="D29" s="1">
         <v>43643.567384259259</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="F29" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B30" s="9">
+        <v>4</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="D30" s="10">
         <v>43643.583333333336</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="F30" s="8" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>486</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B31" s="4">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>800</v>
+      </c>
+      <c r="D31" s="1">
         <v>43643.594780092593</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="F31" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>540</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B32" s="4">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>801</v>
+      </c>
+      <c r="D32" s="1">
         <v>43643.647314814814</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="F32" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>544</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B33" s="4">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>775</v>
+      </c>
+      <c r="D33" s="1">
         <v>43643.651446759257</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="F33" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>556</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B34" s="4">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>802</v>
+      </c>
+      <c r="D34" s="1">
         <v>43643.664212962962</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="F34" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>560</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B35" s="4">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>803</v>
+      </c>
+      <c r="D35" s="1">
         <v>43643.667534722219</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="F35" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>562</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B36" s="4">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>804</v>
+      </c>
+      <c r="D36" s="1">
         <v>43643.669791666667</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="F36" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>578</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B37" s="4">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>805</v>
+      </c>
+      <c r="D37" s="1">
         <v>43643.686701388891</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="F37" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>598</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B38" s="4">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>806</v>
+      </c>
+      <c r="D38" s="1">
         <v>43643.705509259256</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="F38" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>604</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B39" s="4">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>807</v>
+      </c>
+      <c r="D39" s="1">
         <v>43643.712152777778</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="F39" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>630</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B40" s="4">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>808</v>
+      </c>
+      <c r="D40" s="1">
         <v>43643.736747685187</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="F40" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>636</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>809</v>
+      </c>
+      <c r="D41" s="1">
         <v>43643.743125000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="F41" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>666</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B42" s="4">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>810</v>
+      </c>
+      <c r="D42" s="1">
         <v>43643.771620370368</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="F42" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>676</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B43" s="4">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>811</v>
+      </c>
+      <c r="D43" s="1">
         <v>43643.784120370372</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="F43" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>680</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B44" s="4">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>812</v>
+      </c>
+      <c r="D44" s="1">
         <v>43643.788564814815</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="F44" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>712</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B45" s="4">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>813</v>
+      </c>
+      <c r="D45" s="1">
         <v>43643.818460648145</v>
+      </c>
+      <c r="F45" t="s">
+        <v>814</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DEF150-D7DF-6B4A-ABBD-02266A0B69BF}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Reconstruct the file structure
</commit_message>
<xml_diff>
--- a/result_handler/results.xlsx
+++ b/result_handler/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lwyeluo/Workspaces/lab-project/browser/tim-evaluate/result_handler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A5071C-F9A8-0242-8C91-E5C275964BAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375925AF-5406-EE46-8D15-8B4FE0D7DE4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="3" xr2:uid="{A38FA40B-9AA0-234E-B7A1-9A1E5346C45F}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="2" xr2:uid="{A38FA40B-9AA0-234E-B7A1-9A1E5346C45F}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,7 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">distribution!$A$2:$A$19</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">distribution!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">distribution!$B$2:$B$19</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">distribution!$C$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">distribution!$C$2:$C$19</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">distribution!$A$2:$A$19</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">distribution!$B$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">distribution!$B$2:$B$19</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">distribution!$C$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">distribution!$C$2:$C$19</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">distribution!$B$2:$B$19</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">distribution!$A$2:$A$19</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">distribution!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">distribution!$B$2:$B$19</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">distribution!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">distribution!$C$2:$C$19</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">distribution!$A$2:$A$19</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">distribution!$B$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -6711,15 +6696,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4432300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>4508500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30838,7 +30823,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31191,8 +31176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDC9EFE-7FAE-1341-9EA9-E8B8A6EB11B7}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31974,7 +31959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DEF150-D7DF-6B4A-ABBD-02266A0B69BF}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>

</xml_diff>